<commit_message>
Setup transfers as numbers
This module is working perfectly fine with the model behaving as
expected
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_model_simple(counterfactual).xlsx
+++ b/tests/databooks/databook_model_simple(counterfactual).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -545,7 +545,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,12 +777,11 @@
         <f>IF('Transfer Definitions'!C6="y",'Population Definitions'!$A$3,"")</f>
         <v/>
       </c>
-      <c r="D2" t="str">
-        <f>IF(A2&lt;&gt;"...","Fraction","")</f>
-        <v/>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
       <c r="E2" t="str">
-        <f>IF(A2&lt;&gt;"...",IF(SUMPRODUCT(--(G2:V2&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <f>IF(A2&lt;&gt;"...",IF(SUMPRODUCT(--(G2:V2&lt;&gt;""))=0,0.1,"N.A."),"")</f>
         <v/>
       </c>
       <c r="F2" t="str">
@@ -916,10 +915,10 @@
         <v/>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" t="str">
-        <f>IF(A7&lt;&gt;"...",IF(SUMPRODUCT(--(G7:V7&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <f>IF(A7&lt;&gt;"...",IF(SUMPRODUCT(--(G7:V7&lt;&gt;""))=0,0.1,"N.A."),"")</f>
         <v/>
       </c>
       <c r="F7" t="str">

</xml_diff>